<commit_message>
add a prototype of analysis description. i added a context description, problem definition and a funtional requirements. all of them are in spanish and would change because i want to improve redaction. Also, i miss write them in english.
</commit_message>
<xml_diff>
--- a/Doc/following analysis parts.xlsx
+++ b/Doc/following analysis parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\semestre\AED\Workspace\Laboratory-1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CCE86B37-09B7-48D7-9EDC-DFB38FD110C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8C33A662-8E1E-4498-A6FC-678C2F3D020E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{9CCE6E77-F9A5-4118-9822-9A5D0A22CF43}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="2" xr2:uid="{9CCE6E77-F9A5-4118-9822-9A5D0A22CF43}"/>
   </bookViews>
   <sheets>
     <sheet name="TOTAL" sheetId="15" r:id="rId1"/>
@@ -573,24 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -634,6 +616,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -956,8 +956,8 @@
   </sheetPr>
   <dimension ref="D3:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,11 +969,11 @@
   <sheetData>
     <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="4:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="4" t="s">
@@ -1000,7 +1000,7 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="18">
         <f>IF(Analysis!F11=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1011,14 +1011,14 @@
     </row>
     <row r="7" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="5">
-        <f t="shared" ref="D7:D10" si="0">1/$E$13</f>
+        <f t="shared" ref="D7:D9" si="0">1/$E$13</f>
         <v>0.25</v>
       </c>
       <c r="E7" s="2">
         <f>E6+1</f>
         <v>2</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="18">
         <f ca="1">IF(Desing!F11=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1033,10 +1033,10 @@
         <v>0.25</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" ref="E8:E10" si="1">E7+1</f>
+        <f t="shared" ref="E8:E9" si="1">E7+1</f>
         <v>3</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="18">
         <f>IF('Desing''s implementation'!F14=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1054,7 +1054,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="18">
         <f>IF('Desing''s implementation'!F15=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1064,20 +1064,20 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="22"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="14"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
@@ -1091,7 +1091,7 @@
         <f ca="1">SUMPRODUCT(D6:D10,F6:F10)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1120,11 +1120,11 @@
   <sheetData>
     <row r="1" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="4" t="s">
@@ -1151,7 +1151,7 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="18">
         <f>IF('Stage 4'!E12=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1171,7 +1171,7 @@
         <f>E4+1</f>
         <v>2</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="18">
         <f>IF('Stage 5'!E10=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1191,7 +1191,7 @@
         <f t="shared" ref="E6:E7" si="0">E5+1</f>
         <v>3</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="18">
         <f>IF('Stage 5'!E11=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1209,7 +1209,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="18">
         <f>IF('Stage 5'!E12=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1229,7 +1229,7 @@
         <f>E7+1</f>
         <v>5</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="18">
         <f>IF('Stage 5'!E13=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1239,34 +1239,34 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="22"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="22"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G12" s="14"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
@@ -1280,7 +1280,7 @@
         <f>SUMPRODUCT(D4:D8,F4:F8)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1298,7 +1298,7 @@
   <dimension ref="D1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:H11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,11 +1310,11 @@
   <sheetData>
     <row r="1" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="4" t="s">
@@ -1341,7 +1341,7 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="18">
         <f>IF('Stage 1'!F10=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1359,7 +1359,7 @@
         <f>E4+1</f>
         <v>2</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="18">
         <f>IF('Stage 2'!E15=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1377,7 +1377,7 @@
         <f t="shared" ref="E6:E8" si="0">E5+1</f>
         <v>3</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="18">
         <f>IF('Stage 3'!E17=1,1,0)</f>
         <v>0</v>
       </c>
@@ -1395,13 +1395,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F7" s="25">
-        <v>0</v>
-      </c>
-      <c r="G7" s="23" t="s">
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1414,24 +1414,24 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F8" s="25">
-        <v>0</v>
-      </c>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="19">
+        <v>0</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="14"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="14"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
@@ -1445,43 +1445,43 @@
         <f>SUMPRODUCT(D4:D8,F4:F8)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="14"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="14"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1499,8 +1499,8 @@
   </sheetPr>
   <dimension ref="D2:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,11 +1514,11 @@
   <sheetData>
     <row r="2" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:8" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
@@ -1546,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
@@ -1557,14 +1557,14 @@
     </row>
     <row r="6" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="5">
-        <f t="shared" ref="D6:D7" si="0">1/$E$10</f>
+        <f t="shared" ref="D6" si="0">1/$E$10</f>
         <v>0.25</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
@@ -1582,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>15</v>
@@ -1596,7 +1596,7 @@
         <f>1/$E$10</f>
         <v>0.25</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="12">
         <v>4</v>
       </c>
       <c r="F8" s="2">
@@ -1605,16 +1605,16 @@
       <c r="G8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="16"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
@@ -1626,31 +1626,31 @@
       </c>
       <c r="F10" s="5">
         <f>SUMPRODUCT(D5:D8,F5:F8)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="16"/>
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="16"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="16"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="13"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D14" s="6"/>
@@ -1684,11 +1684,11 @@
   <sheetData>
     <row r="2" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
@@ -1745,7 +1745,7 @@
     </row>
     <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="5">
-        <f t="shared" ref="C7:C12" si="0">1/$D$15</f>
+        <f t="shared" ref="C7:C10" si="0">1/$D$15</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="D7" s="2">
@@ -1775,7 +1775,7 @@
       <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1809,30 +1809,30 @@
       <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="16"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1875,11 +1875,11 @@
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -1966,42 +1966,42 @@
       <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="19"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="22"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2044,11 +2044,11 @@
   <sheetData>
     <row r="1" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:8" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="4" t="s">
@@ -2075,7 +2075,7 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="18">
         <f>IF('Stage 4'!E12=1,1,0)</f>
         <v>0</v>
       </c>
@@ -2093,7 +2093,7 @@
         <f>E4+1</f>
         <v>2</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="18">
         <f>IF('Stage 5'!E13=1,1,0)</f>
         <v>0</v>
       </c>
@@ -2111,7 +2111,7 @@
         <f t="shared" ref="E6:E8" si="0">E5+1</f>
         <v>3</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="18">
         <f>IF('Stage 6'!E12=1,1,0)</f>
         <v>0</v>
       </c>
@@ -2129,13 +2129,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F7" s="25">
-        <v>0</v>
-      </c>
-      <c r="G7" s="23" t="s">
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2148,24 +2148,24 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F8" s="25">
-        <v>0</v>
-      </c>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="19">
+        <v>0</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="14"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="14"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
@@ -2179,7 +2179,7 @@
         <f ca="1">SUMPRODUCT(D4:D8,F4:F8)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2208,11 +2208,11 @@
   <sheetData>
     <row r="3" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -2230,7 +2230,7 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="22" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2291,7 +2291,7 @@
       <c r="G8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
@@ -2308,7 +2308,7 @@
       <c r="F9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="13" t="s">
         <v>56</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -2330,17 +2330,17 @@
       <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="13" t="s">
         <v>61</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="16"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
@@ -2354,8 +2354,8 @@
         <f>SUMPRODUCT(C6:C10,E6:E10)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2387,11 +2387,11 @@
   <sheetData>
     <row r="3" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -2409,13 +2409,13 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5">
-        <f>1/$D$13</f>
+        <f t="shared" ref="C6:C11" si="0">1/$D$13</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="D6" s="2">
@@ -2434,7 +2434,7 @@
     </row>
     <row r="7" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="5">
-        <f>1/$D$13</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D7" s="2">
@@ -2450,15 +2450,15 @@
       <c r="G7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
-        <f>1/$D$13</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" ref="D8:D10" si="0">D7+1</f>
+        <f t="shared" ref="D8:D10" si="1">D7+1</f>
         <v>3</v>
       </c>
       <c r="E8" s="2">
@@ -2472,11 +2472,11 @@
     </row>
     <row r="9" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
-        <f>1/$D$13</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E9" s="2">
@@ -2488,15 +2488,15 @@
       <c r="G9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
-        <f>1/$D$13</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E10" s="2">
@@ -2514,7 +2514,7 @@
     </row>
     <row r="11" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
-        <f>1/$D$13</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D11" s="2">
@@ -2527,17 +2527,17 @@
       <c r="F11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="13" t="s">
         <v>71</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
@@ -2551,8 +2551,8 @@
         <f>SUMPRODUCT(C6:C11,E6:E11)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2583,13 +2583,13 @@
   <sheetData>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -2607,10 +2607,10 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="21" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2634,7 +2634,7 @@
       <c r="H6" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="11" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2681,7 +2681,7 @@
       <c r="H8" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="11" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2700,13 +2700,13 @@
       <c r="F9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="13" t="s">
         <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2725,22 +2725,22 @@
       <c r="F10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="H10" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="16"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
@@ -2754,8 +2754,8 @@
         <f>SUMPRODUCT(C6:C10,E6:E10)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>